<commit_message>
Linearisation and contribution statement
Made the A matrix with Faris
</commit_message>
<xml_diff>
--- a/MXB226GroupProjectContributions2019.xlsx
+++ b/MXB226GroupProjectContributions2019.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21328"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MELTUser.QUTAD\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jean-Luc\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96658C2F-1CED-4412-9BD2-79D55E81DF18}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="420" windowWidth="22980" windowHeight="10185" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Code" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="51">
   <si>
     <t>Packed storage</t>
   </si>
@@ -193,11 +194,17 @@
   <si>
     <t>Discussion of resultant matrix</t>
   </si>
+  <si>
+    <t>Jean-Luc</t>
+  </si>
+  <si>
+    <t>Azure, Faris, Jean-luc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -579,7 +586,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -771,11 +778,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +862,9 @@
       <c r="B8" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="3"/>
+      <c r="C8" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
       <c r="F8" s="9" t="s">
@@ -891,7 +900,9 @@
       <c r="B10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3" t="s">
+        <v>50</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
     </row>

</xml_diff>